<commit_message>
Jsave fill the //
</commit_message>
<xml_diff>
--- a/out/production/FIT5136_Team18/sample missionToMars data.xlsx
+++ b/out/production/FIT5136_Team18/sample missionToMars data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arvindkaur/Desktop/FIT5136/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe/IdeaProjects/FIT5136_Team18/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75EA7FF-7AEF-744A-A97A-7D4BF1A2F9A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF27810-239C-6344-B612-C2364F057BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{A04EE760-A0D7-0F4F-BBD2-B5313B5E8A43}"/>
+    <workbookView xWindow="7020" yWindow="1780" windowWidth="23740" windowHeight="17860" activeTab="1" xr2:uid="{A04EE760-A0D7-0F4F-BBD2-B5313B5E8A43}"/>
   </bookViews>
   <sheets>
     <sheet name="missionCoordinators" sheetId="7" r:id="rId1"/>
@@ -4728,8 +4728,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5869,14 +5872,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC397505-3C07-C748-AD52-CD59FD015889}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="47.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B1" t="s">
@@ -5891,7 +5908,7 @@
       <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G1" t="s">
@@ -5918,7 +5935,7 @@
       <c r="N1" t="s">
         <v>115</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>116</v>
       </c>
       <c r="P1" t="s">
@@ -5929,7 +5946,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2176</v>
       </c>
       <c r="B2" t="s">
@@ -5944,7 +5961,7 @@
       <c r="E2" t="s">
         <v>122</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>85200</v>
       </c>
       <c r="G2" t="s">
@@ -5979,7 +5996,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2178</v>
       </c>
       <c r="B3" t="s">
@@ -5994,7 +6011,7 @@
       <c r="E3" t="s">
         <v>136</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>18722</v>
       </c>
       <c r="G3" t="s">
@@ -6018,7 +6035,7 @@
       <c r="M3" t="s">
         <v>142</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="P3" t="s">
@@ -6029,7 +6046,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2180</v>
       </c>
       <c r="B4" t="s">
@@ -6044,7 +6061,7 @@
       <c r="E4" t="s">
         <v>148</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>149</v>
       </c>
       <c r="G4" t="s">
@@ -6065,7 +6082,7 @@
       <c r="L4" t="s">
         <v>141</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P4" t="s">
@@ -6076,7 +6093,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2182</v>
       </c>
       <c r="B5" t="s">
@@ -6091,7 +6108,7 @@
       <c r="E5" t="s">
         <v>161</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>38520</v>
       </c>
       <c r="G5" t="s">
@@ -6118,7 +6135,7 @@
       <c r="N5" t="s">
         <v>167</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="1" t="s">
         <v>168</v>
       </c>
       <c r="P5" t="s">
@@ -6129,7 +6146,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>2184</v>
       </c>
       <c r="B6" t="s">
@@ -6144,7 +6161,7 @@
       <c r="E6" t="s">
         <v>173</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>174</v>
       </c>
       <c r="G6" t="s">
@@ -6168,7 +6185,7 @@
       <c r="M6" t="s">
         <v>178</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1" t="s">
         <v>179</v>
       </c>
       <c r="P6" t="s">
@@ -6179,7 +6196,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>2186</v>
       </c>
       <c r="B7" t="s">
@@ -6194,7 +6211,7 @@
       <c r="E7" t="s">
         <v>184</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>6284</v>
       </c>
       <c r="G7" t="s">
@@ -6226,7 +6243,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>2188</v>
       </c>
       <c r="B8" t="s">
@@ -6241,7 +6258,7 @@
       <c r="E8" t="s">
         <v>193</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>23221</v>
       </c>
       <c r="G8" t="s">
@@ -6276,7 +6293,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>2190</v>
       </c>
       <c r="B9" t="s">
@@ -6291,7 +6308,7 @@
       <c r="E9" t="s">
         <v>202</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="G9" t="s">
@@ -6318,7 +6335,7 @@
       <c r="N9" t="s">
         <v>207</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="1" t="s">
         <v>208</v>
       </c>
       <c r="P9" t="s">
@@ -6326,7 +6343,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>2192</v>
       </c>
       <c r="B10" t="s">
@@ -6341,7 +6358,7 @@
       <c r="E10" t="s">
         <v>213</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>214</v>
       </c>
       <c r="G10" t="s">
@@ -6373,7 +6390,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>2194</v>
       </c>
       <c r="B11" t="s">
@@ -6388,7 +6405,7 @@
       <c r="E11" t="s">
         <v>222</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>32735</v>
       </c>
       <c r="G11" t="s">
@@ -6417,7 +6434,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>2196</v>
       </c>
       <c r="B12" t="s">
@@ -6432,7 +6449,7 @@
       <c r="E12" t="s">
         <v>230</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>554397</v>
       </c>
       <c r="G12" t="s">
@@ -6456,7 +6473,7 @@
       <c r="M12" t="s">
         <v>234</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P12" t="s">
@@ -6464,7 +6481,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>2198</v>
       </c>
       <c r="B13" t="s">
@@ -6479,7 +6496,7 @@
       <c r="E13" t="s">
         <v>239</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>5371</v>
       </c>
       <c r="G13" t="s">
@@ -6506,7 +6523,7 @@
       <c r="N13" t="s">
         <v>244</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="1" t="s">
         <v>245</v>
       </c>
       <c r="P13" t="s">
@@ -6517,7 +6534,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>2200</v>
       </c>
       <c r="B14" t="s">
@@ -6532,7 +6549,7 @@
       <c r="E14" t="s">
         <v>250</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G14" t="s">
@@ -6559,7 +6576,7 @@
       <c r="N14" t="s">
         <v>255</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="1" t="s">
         <v>256</v>
       </c>
       <c r="P14" t="s">
@@ -6570,7 +6587,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>2202</v>
       </c>
       <c r="B15" t="s">
@@ -6585,7 +6602,7 @@
       <c r="E15" t="s">
         <v>261</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>48128</v>
       </c>
       <c r="G15" t="s">
@@ -6612,7 +6629,7 @@
       <c r="N15" t="s">
         <v>265</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="1" t="s">
         <v>266</v>
       </c>
       <c r="P15" t="s">
@@ -6623,7 +6640,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>2204</v>
       </c>
       <c r="B16" t="s">
@@ -6638,7 +6655,7 @@
       <c r="E16" t="s">
         <v>271</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>8442</v>
       </c>
       <c r="G16" t="s">
@@ -6665,7 +6682,7 @@
       <c r="N16" t="s">
         <v>276</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="1" t="s">
         <v>277</v>
       </c>
       <c r="P16" t="s">
@@ -6676,7 +6693,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>2206</v>
       </c>
       <c r="B17" t="s">
@@ -6691,7 +6708,7 @@
       <c r="E17" t="s">
         <v>282</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>20930</v>
       </c>
       <c r="G17" t="s">
@@ -6718,7 +6735,7 @@
       <c r="N17" t="s">
         <v>286</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="1" t="s">
         <v>287</v>
       </c>
       <c r="P17" t="s">
@@ -6729,7 +6746,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>2208</v>
       </c>
       <c r="B18" t="s">
@@ -6744,7 +6761,7 @@
       <c r="E18" t="s">
         <v>292</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>760305</v>
       </c>
       <c r="G18" t="s">
@@ -6765,7 +6782,7 @@
       <c r="L18" t="s">
         <v>187</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="1" t="s">
         <v>295</v>
       </c>
       <c r="P18" t="s">
@@ -6776,7 +6793,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>2210</v>
       </c>
       <c r="B19" t="s">
@@ -6791,7 +6808,7 @@
       <c r="E19" t="s">
         <v>300</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>37844</v>
       </c>
       <c r="G19" t="s">
@@ -6826,7 +6843,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>2212</v>
       </c>
       <c r="B20" t="s">
@@ -6841,7 +6858,7 @@
       <c r="E20" t="s">
         <v>308</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>79604</v>
       </c>
       <c r="G20" t="s">
@@ -6868,7 +6885,7 @@
       <c r="N20" t="s">
         <v>312</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="1" t="s">
         <v>313</v>
       </c>
       <c r="P20" t="s">
@@ -6879,7 +6896,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>2214</v>
       </c>
       <c r="B21" t="s">
@@ -6894,7 +6911,7 @@
       <c r="E21" t="s">
         <v>318</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>1061</v>
       </c>
       <c r="G21" t="s">
@@ -6921,7 +6938,7 @@
       <c r="N21" t="s">
         <v>322</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="1" t="s">
         <v>323</v>
       </c>
       <c r="P21" t="s">
@@ -6932,7 +6949,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>2216</v>
       </c>
       <c r="B22" t="s">
@@ -6947,7 +6964,7 @@
       <c r="E22" t="s">
         <v>328</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>281038</v>
       </c>
       <c r="G22" t="s">
@@ -6971,7 +6988,7 @@
       <c r="M22" t="s">
         <v>311</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="1" t="s">
         <v>331</v>
       </c>
       <c r="P22" t="s">
@@ -6982,7 +6999,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>2218</v>
       </c>
       <c r="B23" t="s">
@@ -6997,7 +7014,7 @@
       <c r="E23" t="s">
         <v>336</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>337</v>
       </c>
       <c r="G23" t="s">
@@ -7024,7 +7041,7 @@
       <c r="N23" t="s">
         <v>341</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P23" t="s">
@@ -7032,7 +7049,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>2220</v>
       </c>
       <c r="B24" t="s">
@@ -7047,7 +7064,7 @@
       <c r="E24" t="s">
         <v>346</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>17393</v>
       </c>
       <c r="G24" t="s">
@@ -7074,7 +7091,7 @@
       <c r="N24" t="s">
         <v>349</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="1" t="s">
         <v>350</v>
       </c>
       <c r="P24" t="s">
@@ -7085,7 +7102,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>2222</v>
       </c>
       <c r="B25" t="s">
@@ -7100,7 +7117,7 @@
       <c r="E25" t="s">
         <v>355</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>356</v>
       </c>
       <c r="G25" t="s">
@@ -7135,7 +7152,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>2224</v>
       </c>
       <c r="B26" t="s">
@@ -7150,7 +7167,7 @@
       <c r="E26" t="s">
         <v>365</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>366</v>
       </c>
       <c r="G26" t="s">
@@ -7185,7 +7202,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>2226</v>
       </c>
       <c r="B27" t="s">
@@ -7200,7 +7217,7 @@
       <c r="E27" t="s">
         <v>374</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>876014</v>
       </c>
       <c r="G27" t="s">
@@ -7224,7 +7241,7 @@
       <c r="M27" t="s">
         <v>377</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="1" t="s">
         <v>378</v>
       </c>
       <c r="P27" t="s">
@@ -7235,7 +7252,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>2228</v>
       </c>
       <c r="B28" t="s">
@@ -7250,7 +7267,7 @@
       <c r="E28" t="s">
         <v>383</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>4854</v>
       </c>
       <c r="G28" t="s">
@@ -7271,7 +7288,7 @@
       <c r="L28" t="s">
         <v>187</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="1" t="s">
         <v>386</v>
       </c>
       <c r="P28" t="s">
@@ -7282,7 +7299,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>2230</v>
       </c>
       <c r="B29" t="s">
@@ -7297,7 +7314,7 @@
       <c r="E29" t="s">
         <v>391</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>3564</v>
       </c>
       <c r="G29" t="s">
@@ -7323,7 +7340,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>2232</v>
       </c>
       <c r="B30" t="s">
@@ -7338,7 +7355,7 @@
       <c r="E30" t="s">
         <v>397</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>6486</v>
       </c>
       <c r="G30" t="s">
@@ -7370,7 +7387,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>2234</v>
       </c>
       <c r="B31" t="s">
@@ -7385,7 +7402,7 @@
       <c r="E31" t="s">
         <v>405</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>6740</v>
       </c>
       <c r="G31" t="s">
@@ -7412,7 +7429,7 @@
       <c r="N31" t="s">
         <v>409</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31" s="1" t="s">
         <v>410</v>
       </c>
       <c r="P31" t="s">
@@ -7423,7 +7440,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>2236</v>
       </c>
       <c r="B32" t="s">
@@ -7438,7 +7455,7 @@
       <c r="E32" t="s">
         <v>415</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>11209</v>
       </c>
       <c r="G32" t="s">
@@ -7465,7 +7482,7 @@
       <c r="N32" t="s">
         <v>418</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32" s="1" t="s">
         <v>419</v>
       </c>
       <c r="P32" t="s">
@@ -7476,7 +7493,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>2238</v>
       </c>
       <c r="B33" t="s">
@@ -7491,7 +7508,7 @@
       <c r="E33" t="s">
         <v>424</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>348422</v>
       </c>
       <c r="G33" t="s">
@@ -7515,7 +7532,7 @@
       <c r="M33" t="s">
         <v>321</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O33" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P33" t="s">
@@ -7523,7 +7540,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>2240</v>
       </c>
       <c r="B34" t="s">
@@ -7538,7 +7555,7 @@
       <c r="E34" t="s">
         <v>430</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>4128</v>
       </c>
       <c r="G34" t="s">
@@ -7565,7 +7582,7 @@
       <c r="N34" t="s">
         <v>433</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="1" t="s">
         <v>434</v>
       </c>
       <c r="P34" t="s">
@@ -7576,7 +7593,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>2242</v>
       </c>
       <c r="B35" t="s">
@@ -7591,7 +7608,7 @@
       <c r="E35" t="s">
         <v>439</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>10785</v>
       </c>
       <c r="G35" t="s">
@@ -7618,7 +7635,7 @@
       <c r="N35" t="s">
         <v>265</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P35" t="s">
@@ -7629,7 +7646,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>2244</v>
       </c>
       <c r="B36" t="s">
@@ -7644,7 +7661,7 @@
       <c r="E36" t="s">
         <v>446</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>40303</v>
       </c>
       <c r="G36" t="s">
@@ -7676,7 +7693,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>2246</v>
       </c>
       <c r="B37" t="s">
@@ -7691,7 +7708,7 @@
       <c r="E37" t="s">
         <v>452</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>453</v>
       </c>
       <c r="G37" t="s">
@@ -7718,7 +7735,7 @@
       <c r="N37" t="s">
         <v>456</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="1" t="s">
         <v>179</v>
       </c>
       <c r="P37" t="s">
@@ -7729,7 +7746,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>2248</v>
       </c>
       <c r="B38" t="s">
@@ -7744,7 +7761,7 @@
       <c r="E38" t="s">
         <v>461</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>40922</v>
       </c>
       <c r="G38" t="s">
@@ -7779,7 +7796,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>2250</v>
       </c>
       <c r="B39" t="s">
@@ -7794,7 +7811,7 @@
       <c r="E39" t="s">
         <v>469</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>470</v>
       </c>
       <c r="G39" t="s">
@@ -7818,7 +7835,7 @@
       <c r="M39" t="s">
         <v>474</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="1" t="s">
         <v>475</v>
       </c>
       <c r="P39" t="s">
@@ -7829,7 +7846,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>2252</v>
       </c>
       <c r="B40" t="s">
@@ -7844,7 +7861,7 @@
       <c r="E40" t="s">
         <v>480</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>27700</v>
       </c>
       <c r="G40" t="s">
@@ -7871,7 +7888,7 @@
       <c r="N40" t="s">
         <v>483</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O40" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P40" t="s">
@@ -7879,7 +7896,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>2254</v>
       </c>
       <c r="B41" t="s">
@@ -7894,7 +7911,7 @@
       <c r="E41" t="s">
         <v>488</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>725172</v>
       </c>
       <c r="G41" t="s">
@@ -7921,7 +7938,7 @@
       <c r="N41" t="s">
         <v>491</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O41" s="1" t="s">
         <v>492</v>
       </c>
       <c r="P41" t="s">
@@ -7929,7 +7946,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>2256</v>
       </c>
       <c r="B42" t="s">
@@ -7944,7 +7961,7 @@
       <c r="E42" t="s">
         <v>496</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>5577</v>
       </c>
       <c r="G42" t="s">
@@ -7968,7 +7985,7 @@
       <c r="M42" t="s">
         <v>178</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O42" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P42" t="s">
@@ -7979,7 +7996,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>2258</v>
       </c>
       <c r="B43" t="s">
@@ -7994,7 +8011,7 @@
       <c r="E43" t="s">
         <v>504</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>83848</v>
       </c>
       <c r="G43" t="s">
@@ -8021,7 +8038,7 @@
       <c r="N43" t="s">
         <v>349</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O43" s="1" t="s">
         <v>507</v>
       </c>
       <c r="P43" t="s">
@@ -8032,7 +8049,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>2260</v>
       </c>
       <c r="B44" t="s">
@@ -8047,7 +8064,7 @@
       <c r="E44" t="s">
         <v>512</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>8109</v>
       </c>
       <c r="G44" t="s">
@@ -8074,7 +8091,7 @@
       <c r="N44" t="s">
         <v>515</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O44" s="1" t="s">
         <v>516</v>
       </c>
       <c r="P44" t="s">
@@ -8085,7 +8102,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>2262</v>
       </c>
       <c r="B45" t="s">
@@ -8100,7 +8117,7 @@
       <c r="E45" t="s">
         <v>521</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>18558</v>
       </c>
       <c r="G45" t="s">
@@ -8127,7 +8144,7 @@
       <c r="N45" t="s">
         <v>286</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O45" s="1" t="s">
         <v>523</v>
       </c>
       <c r="P45" t="s">
@@ -8138,7 +8155,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>2264</v>
       </c>
       <c r="B46" t="s">
@@ -8153,7 +8170,7 @@
       <c r="E46" t="s">
         <v>528</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>20804</v>
       </c>
       <c r="G46" t="s">
@@ -8180,7 +8197,7 @@
       <c r="N46" t="s">
         <v>531</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="1" t="s">
         <v>532</v>
       </c>
       <c r="P46" t="s">
@@ -8188,7 +8205,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>2266</v>
       </c>
       <c r="B47" t="s">
@@ -8203,7 +8220,7 @@
       <c r="E47" t="s">
         <v>536</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>537</v>
       </c>
       <c r="G47" t="s">
@@ -8235,7 +8252,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>2268</v>
       </c>
       <c r="B48" t="s">
@@ -8250,7 +8267,7 @@
       <c r="E48" t="s">
         <v>543</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>26097</v>
       </c>
       <c r="G48" t="s">
@@ -8279,7 +8296,7 @@
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>2270</v>
       </c>
       <c r="B49" t="s">
@@ -8294,7 +8311,7 @@
       <c r="E49" t="s">
         <v>550</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>27729</v>
       </c>
       <c r="G49" t="s">
@@ -8318,7 +8335,7 @@
       <c r="M49" t="s">
         <v>553</v>
       </c>
-      <c r="O49" t="s">
+      <c r="O49" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P49" t="s">
@@ -8329,7 +8346,7 @@
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>2272</v>
       </c>
       <c r="B50" t="s">
@@ -8344,7 +8361,7 @@
       <c r="E50" t="s">
         <v>558</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>42200</v>
       </c>
       <c r="G50" t="s">
@@ -8379,7 +8396,7 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>2274</v>
       </c>
       <c r="B51" t="s">
@@ -8394,7 +8411,7 @@
       <c r="E51" t="s">
         <v>567</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <v>60617</v>
       </c>
       <c r="G51" t="s">
@@ -8418,7 +8435,7 @@
       <c r="N51" t="s">
         <v>276</v>
       </c>
-      <c r="O51" t="s">
+      <c r="O51" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P51" t="s">
@@ -8429,7 +8446,7 @@
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>2276</v>
       </c>
       <c r="B52" t="s">
@@ -8444,7 +8461,7 @@
       <c r="E52" t="s">
         <v>574</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>77940</v>
       </c>
       <c r="G52" t="s">
@@ -8471,7 +8488,7 @@
       <c r="N52" t="s">
         <v>578</v>
       </c>
-      <c r="O52" t="s">
+      <c r="O52" s="1" t="s">
         <v>579</v>
       </c>
       <c r="P52" t="s">
@@ -8482,7 +8499,7 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>2278</v>
       </c>
       <c r="B53" t="s">
@@ -8497,7 +8514,7 @@
       <c r="E53" t="s">
         <v>584</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <v>722378</v>
       </c>
       <c r="G53" t="s">
@@ -8521,7 +8538,7 @@
       <c r="N53" t="s">
         <v>130</v>
       </c>
-      <c r="O53" t="s">
+      <c r="O53" s="1" t="s">
         <v>587</v>
       </c>
       <c r="P53" t="s">
@@ -8532,7 +8549,7 @@
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>2280</v>
       </c>
       <c r="B54" t="s">
@@ -8547,7 +8564,7 @@
       <c r="E54" t="s">
         <v>592</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <v>5164</v>
       </c>
       <c r="G54" t="s">
@@ -8574,7 +8591,7 @@
       <c r="N54" t="s">
         <v>418</v>
       </c>
-      <c r="O54" t="s">
+      <c r="O54" s="1" t="s">
         <v>594</v>
       </c>
       <c r="P54" t="s">
@@ -8585,7 +8602,7 @@
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>2282</v>
       </c>
       <c r="B55" t="s">
@@ -8600,7 +8617,7 @@
       <c r="E55" t="s">
         <v>598</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>599</v>
       </c>
       <c r="G55" t="s">
@@ -8624,7 +8641,7 @@
       <c r="N55" t="s">
         <v>255</v>
       </c>
-      <c r="O55" t="s">
+      <c r="O55" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P55" t="s">
@@ -8635,7 +8652,7 @@
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>2284</v>
       </c>
       <c r="B56" t="s">
@@ -8650,7 +8667,7 @@
       <c r="E56" t="s">
         <v>606</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>579427</v>
       </c>
       <c r="G56" t="s">
@@ -8677,7 +8694,7 @@
       <c r="N56" t="s">
         <v>609</v>
       </c>
-      <c r="O56" t="s">
+      <c r="O56" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P56" t="s">
@@ -8688,7 +8705,7 @@
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>2286</v>
       </c>
       <c r="B57" t="s">
@@ -8703,7 +8720,7 @@
       <c r="E57" t="s">
         <v>614</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <v>982273</v>
       </c>
       <c r="G57" t="s">
@@ -8730,7 +8747,7 @@
       <c r="N57" t="s">
         <v>418</v>
       </c>
-      <c r="O57" t="s">
+      <c r="O57" s="1" t="s">
         <v>618</v>
       </c>
       <c r="P57" t="s">
@@ -8741,7 +8758,7 @@
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>2288</v>
       </c>
       <c r="B58" t="s">
@@ -8756,7 +8773,7 @@
       <c r="E58" t="s">
         <v>623</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="1" t="s">
         <v>624</v>
       </c>
       <c r="G58" t="s">
@@ -8783,7 +8800,7 @@
       <c r="N58" t="s">
         <v>626</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O58" s="1" t="s">
         <v>627</v>
       </c>
       <c r="P58" t="s">
@@ -8794,7 +8811,7 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>2290</v>
       </c>
       <c r="B59" t="s">
@@ -8809,7 +8826,7 @@
       <c r="E59" t="s">
         <v>632</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>682358</v>
       </c>
       <c r="G59" t="s">
@@ -8833,7 +8850,7 @@
       <c r="N59" t="s">
         <v>286</v>
       </c>
-      <c r="O59" t="s">
+      <c r="O59" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P59" t="s">
@@ -8844,7 +8861,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>2292</v>
       </c>
       <c r="B60" t="s">
@@ -8859,7 +8876,7 @@
       <c r="E60" t="s">
         <v>638</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>639</v>
       </c>
       <c r="G60" t="s">
@@ -8888,7 +8905,7 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>2294</v>
       </c>
       <c r="B61" t="s">
@@ -8903,7 +8920,7 @@
       <c r="E61" t="s">
         <v>646</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>2552</v>
       </c>
       <c r="G61" t="s">
@@ -8927,7 +8944,7 @@
       <c r="M61" t="s">
         <v>648</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O61" s="1" t="s">
         <v>649</v>
       </c>
       <c r="P61" t="s">
@@ -8938,7 +8955,7 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>2296</v>
       </c>
       <c r="B62" t="s">
@@ -8953,7 +8970,7 @@
       <c r="E62" t="s">
         <v>654</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="1" t="s">
         <v>655</v>
       </c>
       <c r="G62" t="s">
@@ -8980,7 +8997,7 @@
       <c r="N62" t="s">
         <v>456</v>
       </c>
-      <c r="O62" t="s">
+      <c r="O62" s="1" t="s">
         <v>658</v>
       </c>
       <c r="P62" t="s">
@@ -8988,7 +9005,7 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>2298</v>
       </c>
       <c r="B63" t="s">
@@ -9003,7 +9020,7 @@
       <c r="E63" t="s">
         <v>662</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <v>39196</v>
       </c>
       <c r="G63" t="s">
@@ -9027,7 +9044,7 @@
       <c r="N63" t="s">
         <v>130</v>
       </c>
-      <c r="O63" t="s">
+      <c r="O63" s="1" t="s">
         <v>665</v>
       </c>
       <c r="P63" t="s">
@@ -9038,7 +9055,7 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>2300</v>
       </c>
       <c r="B64" t="s">
@@ -9053,7 +9070,7 @@
       <c r="E64" t="s">
         <v>670</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="1">
         <v>185366</v>
       </c>
       <c r="G64" t="s">
@@ -9080,7 +9097,7 @@
       <c r="N64" t="s">
         <v>674</v>
       </c>
-      <c r="O64" t="s">
+      <c r="O64" s="1" t="s">
         <v>675</v>
       </c>
       <c r="P64" t="s">
@@ -9091,7 +9108,7 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>2302</v>
       </c>
       <c r="B65" t="s">
@@ -9106,7 +9123,7 @@
       <c r="E65" t="s">
         <v>680</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <v>84558</v>
       </c>
       <c r="G65" t="s">
@@ -9133,7 +9150,7 @@
       <c r="N65" t="s">
         <v>683</v>
       </c>
-      <c r="O65" t="s">
+      <c r="O65" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P65" t="s">
@@ -9144,7 +9161,7 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>2304</v>
       </c>
       <c r="B66" t="s">
@@ -9159,7 +9176,7 @@
       <c r="E66" t="s">
         <v>688</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <v>50100</v>
       </c>
       <c r="G66" t="s">
@@ -9191,7 +9208,7 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>2306</v>
       </c>
       <c r="B67" t="s">
@@ -9206,7 +9223,7 @@
       <c r="E67" t="s">
         <v>696</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="1">
         <v>784335</v>
       </c>
       <c r="G67" t="s">
@@ -9230,7 +9247,7 @@
       <c r="N67" t="s">
         <v>515</v>
       </c>
-      <c r="O67" t="s">
+      <c r="O67" s="1" t="s">
         <v>699</v>
       </c>
       <c r="P67" t="s">
@@ -9238,7 +9255,7 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>2308</v>
       </c>
       <c r="B68" t="s">
@@ -9253,7 +9270,7 @@
       <c r="E68" t="s">
         <v>703</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <v>61400</v>
       </c>
       <c r="G68" t="s">
@@ -9288,7 +9305,7 @@
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>2310</v>
       </c>
       <c r="B69" t="s">
@@ -9303,7 +9320,7 @@
       <c r="E69" t="s">
         <v>711</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="1">
         <v>20800</v>
       </c>
       <c r="G69" t="s">
@@ -9330,7 +9347,7 @@
       <c r="N69" t="s">
         <v>255</v>
       </c>
-      <c r="O69" t="s">
+      <c r="O69" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P69" t="s">
@@ -9341,7 +9358,7 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>2312</v>
       </c>
       <c r="B70" t="s">
@@ -9356,7 +9373,7 @@
       <c r="E70" t="s">
         <v>623</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="1">
         <v>495497</v>
       </c>
       <c r="G70" t="s">
@@ -9380,7 +9397,7 @@
       <c r="N70" t="s">
         <v>719</v>
       </c>
-      <c r="O70" t="s">
+      <c r="O70" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P70" t="s">
@@ -9391,7 +9408,7 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>2314</v>
       </c>
       <c r="B71" t="s">
@@ -9406,7 +9423,7 @@
       <c r="E71" t="s">
         <v>724</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="1">
         <v>30365</v>
       </c>
       <c r="G71" t="s">
@@ -9438,7 +9455,7 @@
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>2316</v>
       </c>
       <c r="B72" t="s">
@@ -9453,7 +9470,7 @@
       <c r="E72" t="s">
         <v>732</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="1">
         <v>647071</v>
       </c>
       <c r="G72" t="s">
@@ -9480,7 +9497,7 @@
       <c r="N72" t="s">
         <v>734</v>
       </c>
-      <c r="O72" t="s">
+      <c r="O72" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P72" t="s">
@@ -9491,7 +9508,7 @@
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>2318</v>
       </c>
       <c r="B73" t="s">
@@ -9506,7 +9523,7 @@
       <c r="E73" t="s">
         <v>739</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="1">
         <v>7801</v>
       </c>
       <c r="G73" t="s">
@@ -9530,7 +9547,7 @@
       <c r="M73" t="s">
         <v>188</v>
       </c>
-      <c r="O73" t="s">
+      <c r="O73" s="1" t="s">
         <v>143</v>
       </c>
       <c r="P73" t="s">
@@ -9541,7 +9558,7 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>2320</v>
       </c>
       <c r="B74" t="s">
@@ -9556,7 +9573,7 @@
       <c r="E74" t="s">
         <v>745</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="1">
         <v>6472</v>
       </c>
       <c r="G74" t="s">
@@ -9582,7 +9599,7 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>2322</v>
       </c>
       <c r="B75" t="s">
@@ -9597,7 +9614,7 @@
       <c r="E75" t="s">
         <v>751</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>752</v>
       </c>
       <c r="G75" t="s">
@@ -9624,7 +9641,7 @@
       <c r="N75" t="s">
         <v>755</v>
       </c>
-      <c r="O75" t="s">
+      <c r="O75" s="1" t="s">
         <v>594</v>
       </c>
       <c r="P75" t="s">
@@ -9635,7 +9652,7 @@
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>2324</v>
       </c>
       <c r="B76" t="s">
@@ -9650,7 +9667,7 @@
       <c r="E76" t="s">
         <v>760</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="1">
         <v>613813</v>
       </c>
       <c r="G76" t="s">
@@ -9677,7 +9694,7 @@
       <c r="N76" t="s">
         <v>418</v>
       </c>
-      <c r="O76" t="s">
+      <c r="O76" s="1" t="s">
         <v>763</v>
       </c>
       <c r="P76" t="s">
@@ -9688,7 +9705,7 @@
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>2326</v>
       </c>
       <c r="B77" t="s">
@@ -9703,7 +9720,7 @@
       <c r="E77" t="s">
         <v>768</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="1">
         <v>21600</v>
       </c>
       <c r="G77" t="s">
@@ -9738,7 +9755,7 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>2328</v>
       </c>
       <c r="B78" t="s">
@@ -9753,7 +9770,7 @@
       <c r="E78" t="s">
         <v>776</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="1">
         <v>22930</v>
       </c>
       <c r="G78" t="s">
@@ -9777,7 +9794,7 @@
       <c r="M78" t="s">
         <v>311</v>
       </c>
-      <c r="O78" t="s">
+      <c r="O78" s="1" t="s">
         <v>618</v>
       </c>
       <c r="P78" t="s">
@@ -9788,7 +9805,7 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>2330</v>
       </c>
       <c r="B79" t="s">
@@ -9803,7 +9820,7 @@
       <c r="E79" t="s">
         <v>783</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="1">
         <v>18648</v>
       </c>
       <c r="G79" t="s">
@@ -9830,7 +9847,7 @@
       <c r="N79" t="s">
         <v>786</v>
       </c>
-      <c r="O79" t="s">
+      <c r="O79" s="1" t="s">
         <v>516</v>
       </c>
       <c r="P79" t="s">
@@ -9841,7 +9858,7 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>2332</v>
       </c>
       <c r="B80" t="s">
@@ -9856,7 +9873,7 @@
       <c r="E80" t="s">
         <v>790</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="1" t="s">
         <v>791</v>
       </c>
       <c r="G80" t="s">
@@ -9885,7 +9902,7 @@
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>2334</v>
       </c>
       <c r="B81" t="s">
@@ -9900,7 +9917,7 @@
       <c r="E81" t="s">
         <v>796</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="1">
         <v>60175</v>
       </c>
       <c r="G81" t="s">
@@ -9932,7 +9949,7 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>2336</v>
       </c>
       <c r="B82" t="s">
@@ -9947,7 +9964,7 @@
       <c r="E82" t="s">
         <v>802</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="1">
         <v>13427</v>
       </c>
       <c r="G82" t="s">
@@ -9971,7 +9988,7 @@
       <c r="M82" t="s">
         <v>805</v>
       </c>
-      <c r="O82" t="s">
+      <c r="O82" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P82" t="s">
@@ -9982,7 +9999,7 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>2338</v>
       </c>
       <c r="B83" t="s">
@@ -9997,7 +10014,7 @@
       <c r="E83" t="s">
         <v>623</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="1" t="s">
         <v>810</v>
       </c>
       <c r="G83" t="s">
@@ -10024,7 +10041,7 @@
       <c r="N83" t="s">
         <v>531</v>
       </c>
-      <c r="O83" t="s">
+      <c r="O83" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P83" t="s">
@@ -10035,7 +10052,7 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>2340</v>
       </c>
       <c r="B84" t="s">
@@ -10050,7 +10067,7 @@
       <c r="E84" t="s">
         <v>817</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="1">
         <v>15388</v>
       </c>
       <c r="G84" t="s">
@@ -10077,7 +10094,7 @@
       <c r="N84" t="s">
         <v>820</v>
       </c>
-      <c r="O84" t="s">
+      <c r="O84" s="1" t="s">
         <v>821</v>
       </c>
       <c r="P84" t="s">
@@ -10088,7 +10105,7 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>2342</v>
       </c>
       <c r="B85" t="s">
@@ -10103,7 +10120,7 @@
       <c r="E85" t="s">
         <v>826</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="1">
         <v>763583</v>
       </c>
       <c r="G85" t="s">
@@ -10130,7 +10147,7 @@
       <c r="N85" t="s">
         <v>829</v>
       </c>
-      <c r="O85" t="s">
+      <c r="O85" s="1" t="s">
         <v>830</v>
       </c>
       <c r="P85" t="s">
@@ -10138,7 +10155,7 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>2344</v>
       </c>
       <c r="B86" t="s">
@@ -10153,7 +10170,7 @@
       <c r="E86" t="s">
         <v>834</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="1">
         <v>21505</v>
       </c>
       <c r="G86" t="s">
@@ -10180,7 +10197,7 @@
       <c r="N86" t="s">
         <v>515</v>
       </c>
-      <c r="O86" t="s">
+      <c r="O86" s="1" t="s">
         <v>837</v>
       </c>
       <c r="P86" t="s">
@@ -10191,7 +10208,7 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>2346</v>
       </c>
       <c r="B87" t="s">
@@ -10206,7 +10223,7 @@
       <c r="E87" t="s">
         <v>842</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="1">
         <v>854349</v>
       </c>
       <c r="G87" t="s">
@@ -10233,7 +10250,7 @@
       <c r="N87" t="s">
         <v>578</v>
       </c>
-      <c r="O87" t="s">
+      <c r="O87" s="1" t="s">
         <v>844</v>
       </c>
       <c r="P87" t="s">
@@ -10244,7 +10261,7 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>2348</v>
       </c>
       <c r="B88" t="s">
@@ -10259,7 +10276,7 @@
       <c r="E88" t="s">
         <v>849</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="1">
         <v>99479</v>
       </c>
       <c r="G88" t="s">
@@ -10286,7 +10303,7 @@
       <c r="N88" t="s">
         <v>276</v>
       </c>
-      <c r="O88" t="s">
+      <c r="O88" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P88" t="s">
@@ -10297,7 +10314,7 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>2350</v>
       </c>
       <c r="B89" t="s">
@@ -10312,7 +10329,7 @@
       <c r="E89" t="s">
         <v>855</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="1">
         <v>39926</v>
       </c>
       <c r="G89" t="s">
@@ -10336,7 +10353,7 @@
       <c r="N89" t="s">
         <v>857</v>
       </c>
-      <c r="O89" t="s">
+      <c r="O89" s="1" t="s">
         <v>858</v>
       </c>
       <c r="P89" t="s">
@@ -10347,7 +10364,7 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>2352</v>
       </c>
       <c r="B90" t="s">
@@ -10362,7 +10379,7 @@
       <c r="E90" t="s">
         <v>863</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="1">
         <v>956033</v>
       </c>
       <c r="G90" t="s">
@@ -10389,7 +10406,7 @@
       <c r="N90" t="s">
         <v>866</v>
       </c>
-      <c r="O90" t="s">
+      <c r="O90" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P90" t="s">
@@ -10400,7 +10417,7 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>2354</v>
       </c>
       <c r="B91" t="s">
@@ -10415,7 +10432,7 @@
       <c r="E91" t="s">
         <v>871</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="1">
         <v>27729</v>
       </c>
       <c r="G91" t="s">
@@ -10442,7 +10459,7 @@
       <c r="N91" t="s">
         <v>873</v>
       </c>
-      <c r="O91" t="s">
+      <c r="O91" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P91" t="s">
@@ -10453,7 +10470,7 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>2356</v>
       </c>
       <c r="B92" t="s">
@@ -10468,7 +10485,7 @@
       <c r="E92" t="s">
         <v>877</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="1">
         <v>16704</v>
       </c>
       <c r="G92" t="s">
@@ -10492,7 +10509,7 @@
       <c r="N92" t="s">
         <v>880</v>
       </c>
-      <c r="O92" t="s">
+      <c r="O92" s="1" t="s">
         <v>287</v>
       </c>
       <c r="P92" t="s">
@@ -10500,7 +10517,7 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>2358</v>
       </c>
       <c r="B93" t="s">
@@ -10515,7 +10532,7 @@
       <c r="E93" t="s">
         <v>884</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="1">
         <v>4932</v>
       </c>
       <c r="G93" t="s">
@@ -10539,7 +10556,7 @@
       <c r="M93" t="s">
         <v>188</v>
       </c>
-      <c r="O93" t="s">
+      <c r="O93" s="1" t="s">
         <v>658</v>
       </c>
       <c r="P93" t="s">
@@ -10550,7 +10567,7 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>2360</v>
       </c>
       <c r="B94" t="s">
@@ -10565,7 +10582,7 @@
       <c r="E94" t="s">
         <v>891</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="1">
         <v>969734</v>
       </c>
       <c r="G94" t="s">
@@ -10600,7 +10617,7 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>2362</v>
       </c>
       <c r="B95" t="s">
@@ -10615,7 +10632,7 @@
       <c r="E95" t="s">
         <v>898</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="1">
         <v>2130</v>
       </c>
       <c r="G95" t="s">
@@ -10642,7 +10659,7 @@
       <c r="N95" t="s">
         <v>515</v>
       </c>
-      <c r="O95" t="s">
+      <c r="O95" s="1" t="s">
         <v>901</v>
       </c>
       <c r="P95" t="s">
@@ -10650,7 +10667,7 @@
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>2364</v>
       </c>
       <c r="B96" t="s">
@@ -10665,7 +10682,7 @@
       <c r="E96" t="s">
         <v>905</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="1">
         <v>8145</v>
       </c>
       <c r="G96" t="s">
@@ -10694,7 +10711,7 @@
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>2366</v>
       </c>
       <c r="B97" t="s">
@@ -10709,7 +10726,7 @@
       <c r="E97" t="s">
         <v>912</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="1" t="s">
         <v>913</v>
       </c>
       <c r="G97" t="s">
@@ -10736,7 +10753,7 @@
       <c r="N97" t="s">
         <v>276</v>
       </c>
-      <c r="O97" t="s">
+      <c r="O97" s="1" t="s">
         <v>916</v>
       </c>
       <c r="P97" t="s">
@@ -10747,7 +10764,7 @@
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>2368</v>
       </c>
       <c r="B98" t="s">
@@ -10762,7 +10779,7 @@
       <c r="E98" t="s">
         <v>921</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="1">
         <v>823823</v>
       </c>
       <c r="G98" t="s">
@@ -10786,7 +10803,7 @@
       <c r="M98" t="s">
         <v>254</v>
       </c>
-      <c r="O98" t="s">
+      <c r="O98" s="1" t="s">
         <v>532</v>
       </c>
       <c r="P98" t="s">
@@ -10797,7 +10814,7 @@
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>2370</v>
       </c>
       <c r="B99" t="s">
@@ -10812,7 +10829,7 @@
       <c r="E99" t="s">
         <v>927</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="1">
         <v>583509</v>
       </c>
       <c r="G99" t="s">
@@ -10836,7 +10853,7 @@
       <c r="M99" t="s">
         <v>196</v>
       </c>
-      <c r="O99" t="s">
+      <c r="O99" s="1" t="s">
         <v>930</v>
       </c>
       <c r="P99" t="s">
@@ -10844,7 +10861,7 @@
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>2372</v>
       </c>
       <c r="B100" t="s">
@@ -10859,7 +10876,7 @@
       <c r="E100" t="s">
         <v>934</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="1">
         <v>588185</v>
       </c>
       <c r="G100" t="s">
@@ -10883,7 +10900,7 @@
       <c r="N100" t="s">
         <v>873</v>
       </c>
-      <c r="O100" t="s">
+      <c r="O100" s="1" t="s">
         <v>937</v>
       </c>
       <c r="P100" t="s">
@@ -10894,7 +10911,7 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>2374</v>
       </c>
       <c r="B101" t="s">
@@ -10909,7 +10926,7 @@
       <c r="E101" t="s">
         <v>942</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="1">
         <v>7053</v>
       </c>
       <c r="G101" t="s">
@@ -10936,7 +10953,7 @@
       <c r="N101" t="s">
         <v>945</v>
       </c>
-      <c r="O101" t="s">
+      <c r="O101" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P101" t="s">
@@ -18670,7 +18687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89A6CDD-DBCC-584C-89E0-70AF5717A48B}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
for testing write method
</commit_message>
<xml_diff>
--- a/out/production/FIT5136_Team18/sample missionToMars data.xlsx
+++ b/out/production/FIT5136_Team18/sample missionToMars data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arvindkaur/Desktop/FIT5136/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoe/IdeaProjects/FIT5136_Team18/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75EA7FF-7AEF-744A-A97A-7D4BF1A2F9A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF27810-239C-6344-B612-C2364F057BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="4" xr2:uid="{A04EE760-A0D7-0F4F-BBD2-B5313B5E8A43}"/>
+    <workbookView xWindow="7020" yWindow="1780" windowWidth="23740" windowHeight="17860" activeTab="1" xr2:uid="{A04EE760-A0D7-0F4F-BBD2-B5313B5E8A43}"/>
   </bookViews>
   <sheets>
     <sheet name="missionCoordinators" sheetId="7" r:id="rId1"/>
@@ -4728,8 +4728,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5869,14 +5872,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC397505-3C07-C748-AD52-CD59FD015889}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="9" width="16.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="47.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B1" t="s">
@@ -5891,7 +5908,7 @@
       <c r="E1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>107</v>
       </c>
       <c r="G1" t="s">
@@ -5918,7 +5935,7 @@
       <c r="N1" t="s">
         <v>115</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>116</v>
       </c>
       <c r="P1" t="s">
@@ -5929,7 +5946,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2176</v>
       </c>
       <c r="B2" t="s">
@@ -5944,7 +5961,7 @@
       <c r="E2" t="s">
         <v>122</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>85200</v>
       </c>
       <c r="G2" t="s">
@@ -5979,7 +5996,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2178</v>
       </c>
       <c r="B3" t="s">
@@ -5994,7 +6011,7 @@
       <c r="E3" t="s">
         <v>136</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>18722</v>
       </c>
       <c r="G3" t="s">
@@ -6018,7 +6035,7 @@
       <c r="M3" t="s">
         <v>142</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="1" t="s">
         <v>143</v>
       </c>
       <c r="P3" t="s">
@@ -6029,7 +6046,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2180</v>
       </c>
       <c r="B4" t="s">
@@ -6044,7 +6061,7 @@
       <c r="E4" t="s">
         <v>148</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>149</v>
       </c>
       <c r="G4" t="s">
@@ -6065,7 +6082,7 @@
       <c r="L4" t="s">
         <v>141</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P4" t="s">
@@ -6076,7 +6093,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>2182</v>
       </c>
       <c r="B5" t="s">
@@ -6091,7 +6108,7 @@
       <c r="E5" t="s">
         <v>161</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>38520</v>
       </c>
       <c r="G5" t="s">
@@ -6118,7 +6135,7 @@
       <c r="N5" t="s">
         <v>167</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="1" t="s">
         <v>168</v>
       </c>
       <c r="P5" t="s">
@@ -6129,7 +6146,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>2184</v>
       </c>
       <c r="B6" t="s">
@@ -6144,7 +6161,7 @@
       <c r="E6" t="s">
         <v>173</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>174</v>
       </c>
       <c r="G6" t="s">
@@ -6168,7 +6185,7 @@
       <c r="M6" t="s">
         <v>178</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="1" t="s">
         <v>179</v>
       </c>
       <c r="P6" t="s">
@@ -6179,7 +6196,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>2186</v>
       </c>
       <c r="B7" t="s">
@@ -6194,7 +6211,7 @@
       <c r="E7" t="s">
         <v>184</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>6284</v>
       </c>
       <c r="G7" t="s">
@@ -6226,7 +6243,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>2188</v>
       </c>
       <c r="B8" t="s">
@@ -6241,7 +6258,7 @@
       <c r="E8" t="s">
         <v>193</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>23221</v>
       </c>
       <c r="G8" t="s">
@@ -6276,7 +6293,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>2190</v>
       </c>
       <c r="B9" t="s">
@@ -6291,7 +6308,7 @@
       <c r="E9" t="s">
         <v>202</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>203</v>
       </c>
       <c r="G9" t="s">
@@ -6318,7 +6335,7 @@
       <c r="N9" t="s">
         <v>207</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="1" t="s">
         <v>208</v>
       </c>
       <c r="P9" t="s">
@@ -6326,7 +6343,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>2192</v>
       </c>
       <c r="B10" t="s">
@@ -6341,7 +6358,7 @@
       <c r="E10" t="s">
         <v>213</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>214</v>
       </c>
       <c r="G10" t="s">
@@ -6373,7 +6390,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>2194</v>
       </c>
       <c r="B11" t="s">
@@ -6388,7 +6405,7 @@
       <c r="E11" t="s">
         <v>222</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>32735</v>
       </c>
       <c r="G11" t="s">
@@ -6417,7 +6434,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>2196</v>
       </c>
       <c r="B12" t="s">
@@ -6432,7 +6449,7 @@
       <c r="E12" t="s">
         <v>230</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>554397</v>
       </c>
       <c r="G12" t="s">
@@ -6456,7 +6473,7 @@
       <c r="M12" t="s">
         <v>234</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P12" t="s">
@@ -6464,7 +6481,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>2198</v>
       </c>
       <c r="B13" t="s">
@@ -6479,7 +6496,7 @@
       <c r="E13" t="s">
         <v>239</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>5371</v>
       </c>
       <c r="G13" t="s">
@@ -6506,7 +6523,7 @@
       <c r="N13" t="s">
         <v>244</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="1" t="s">
         <v>245</v>
       </c>
       <c r="P13" t="s">
@@ -6517,7 +6534,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>2200</v>
       </c>
       <c r="B14" t="s">
@@ -6532,7 +6549,7 @@
       <c r="E14" t="s">
         <v>250</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>251</v>
       </c>
       <c r="G14" t="s">
@@ -6559,7 +6576,7 @@
       <c r="N14" t="s">
         <v>255</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="1" t="s">
         <v>256</v>
       </c>
       <c r="P14" t="s">
@@ -6570,7 +6587,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>2202</v>
       </c>
       <c r="B15" t="s">
@@ -6585,7 +6602,7 @@
       <c r="E15" t="s">
         <v>261</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>48128</v>
       </c>
       <c r="G15" t="s">
@@ -6612,7 +6629,7 @@
       <c r="N15" t="s">
         <v>265</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="1" t="s">
         <v>266</v>
       </c>
       <c r="P15" t="s">
@@ -6623,7 +6640,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>2204</v>
       </c>
       <c r="B16" t="s">
@@ -6638,7 +6655,7 @@
       <c r="E16" t="s">
         <v>271</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>8442</v>
       </c>
       <c r="G16" t="s">
@@ -6665,7 +6682,7 @@
       <c r="N16" t="s">
         <v>276</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="1" t="s">
         <v>277</v>
       </c>
       <c r="P16" t="s">
@@ -6676,7 +6693,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>2206</v>
       </c>
       <c r="B17" t="s">
@@ -6691,7 +6708,7 @@
       <c r="E17" t="s">
         <v>282</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>20930</v>
       </c>
       <c r="G17" t="s">
@@ -6718,7 +6735,7 @@
       <c r="N17" t="s">
         <v>286</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O17" s="1" t="s">
         <v>287</v>
       </c>
       <c r="P17" t="s">
@@ -6729,7 +6746,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>2208</v>
       </c>
       <c r="B18" t="s">
@@ -6744,7 +6761,7 @@
       <c r="E18" t="s">
         <v>292</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>760305</v>
       </c>
       <c r="G18" t="s">
@@ -6765,7 +6782,7 @@
       <c r="L18" t="s">
         <v>187</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="1" t="s">
         <v>295</v>
       </c>
       <c r="P18" t="s">
@@ -6776,7 +6793,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>2210</v>
       </c>
       <c r="B19" t="s">
@@ -6791,7 +6808,7 @@
       <c r="E19" t="s">
         <v>300</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>37844</v>
       </c>
       <c r="G19" t="s">
@@ -6826,7 +6843,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>2212</v>
       </c>
       <c r="B20" t="s">
@@ -6841,7 +6858,7 @@
       <c r="E20" t="s">
         <v>308</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>79604</v>
       </c>
       <c r="G20" t="s">
@@ -6868,7 +6885,7 @@
       <c r="N20" t="s">
         <v>312</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="1" t="s">
         <v>313</v>
       </c>
       <c r="P20" t="s">
@@ -6879,7 +6896,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>2214</v>
       </c>
       <c r="B21" t="s">
@@ -6894,7 +6911,7 @@
       <c r="E21" t="s">
         <v>318</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>1061</v>
       </c>
       <c r="G21" t="s">
@@ -6921,7 +6938,7 @@
       <c r="N21" t="s">
         <v>322</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="1" t="s">
         <v>323</v>
       </c>
       <c r="P21" t="s">
@@ -6932,7 +6949,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>2216</v>
       </c>
       <c r="B22" t="s">
@@ -6947,7 +6964,7 @@
       <c r="E22" t="s">
         <v>328</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>281038</v>
       </c>
       <c r="G22" t="s">
@@ -6971,7 +6988,7 @@
       <c r="M22" t="s">
         <v>311</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="1" t="s">
         <v>331</v>
       </c>
       <c r="P22" t="s">
@@ -6982,7 +6999,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>2218</v>
       </c>
       <c r="B23" t="s">
@@ -6997,7 +7014,7 @@
       <c r="E23" t="s">
         <v>336</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="1" t="s">
         <v>337</v>
       </c>
       <c r="G23" t="s">
@@ -7024,7 +7041,7 @@
       <c r="N23" t="s">
         <v>341</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P23" t="s">
@@ -7032,7 +7049,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>2220</v>
       </c>
       <c r="B24" t="s">
@@ -7047,7 +7064,7 @@
       <c r="E24" t="s">
         <v>346</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>17393</v>
       </c>
       <c r="G24" t="s">
@@ -7074,7 +7091,7 @@
       <c r="N24" t="s">
         <v>349</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="1" t="s">
         <v>350</v>
       </c>
       <c r="P24" t="s">
@@ -7085,7 +7102,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>2222</v>
       </c>
       <c r="B25" t="s">
@@ -7100,7 +7117,7 @@
       <c r="E25" t="s">
         <v>355</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>356</v>
       </c>
       <c r="G25" t="s">
@@ -7135,7 +7152,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>2224</v>
       </c>
       <c r="B26" t="s">
@@ -7150,7 +7167,7 @@
       <c r="E26" t="s">
         <v>365</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>366</v>
       </c>
       <c r="G26" t="s">
@@ -7185,7 +7202,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>2226</v>
       </c>
       <c r="B27" t="s">
@@ -7200,7 +7217,7 @@
       <c r="E27" t="s">
         <v>374</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>876014</v>
       </c>
       <c r="G27" t="s">
@@ -7224,7 +7241,7 @@
       <c r="M27" t="s">
         <v>377</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="1" t="s">
         <v>378</v>
       </c>
       <c r="P27" t="s">
@@ -7235,7 +7252,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>2228</v>
       </c>
       <c r="B28" t="s">
@@ -7250,7 +7267,7 @@
       <c r="E28" t="s">
         <v>383</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>4854</v>
       </c>
       <c r="G28" t="s">
@@ -7271,7 +7288,7 @@
       <c r="L28" t="s">
         <v>187</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="1" t="s">
         <v>386</v>
       </c>
       <c r="P28" t="s">
@@ -7282,7 +7299,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>2230</v>
       </c>
       <c r="B29" t="s">
@@ -7297,7 +7314,7 @@
       <c r="E29" t="s">
         <v>391</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>3564</v>
       </c>
       <c r="G29" t="s">
@@ -7323,7 +7340,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>2232</v>
       </c>
       <c r="B30" t="s">
@@ -7338,7 +7355,7 @@
       <c r="E30" t="s">
         <v>397</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>6486</v>
       </c>
       <c r="G30" t="s">
@@ -7370,7 +7387,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>2234</v>
       </c>
       <c r="B31" t="s">
@@ -7385,7 +7402,7 @@
       <c r="E31" t="s">
         <v>405</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>6740</v>
       </c>
       <c r="G31" t="s">
@@ -7412,7 +7429,7 @@
       <c r="N31" t="s">
         <v>409</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31" s="1" t="s">
         <v>410</v>
       </c>
       <c r="P31" t="s">
@@ -7423,7 +7440,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>2236</v>
       </c>
       <c r="B32" t="s">
@@ -7438,7 +7455,7 @@
       <c r="E32" t="s">
         <v>415</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>11209</v>
       </c>
       <c r="G32" t="s">
@@ -7465,7 +7482,7 @@
       <c r="N32" t="s">
         <v>418</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32" s="1" t="s">
         <v>419</v>
       </c>
       <c r="P32" t="s">
@@ -7476,7 +7493,7 @@
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>2238</v>
       </c>
       <c r="B33" t="s">
@@ -7491,7 +7508,7 @@
       <c r="E33" t="s">
         <v>424</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>348422</v>
       </c>
       <c r="G33" t="s">
@@ -7515,7 +7532,7 @@
       <c r="M33" t="s">
         <v>321</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O33" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P33" t="s">
@@ -7523,7 +7540,7 @@
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>2240</v>
       </c>
       <c r="B34" t="s">
@@ -7538,7 +7555,7 @@
       <c r="E34" t="s">
         <v>430</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>4128</v>
       </c>
       <c r="G34" t="s">
@@ -7565,7 +7582,7 @@
       <c r="N34" t="s">
         <v>433</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="1" t="s">
         <v>434</v>
       </c>
       <c r="P34" t="s">
@@ -7576,7 +7593,7 @@
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>2242</v>
       </c>
       <c r="B35" t="s">
@@ -7591,7 +7608,7 @@
       <c r="E35" t="s">
         <v>439</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>10785</v>
       </c>
       <c r="G35" t="s">
@@ -7618,7 +7635,7 @@
       <c r="N35" t="s">
         <v>265</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P35" t="s">
@@ -7629,7 +7646,7 @@
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>2244</v>
       </c>
       <c r="B36" t="s">
@@ -7644,7 +7661,7 @@
       <c r="E36" t="s">
         <v>446</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>40303</v>
       </c>
       <c r="G36" t="s">
@@ -7676,7 +7693,7 @@
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>2246</v>
       </c>
       <c r="B37" t="s">
@@ -7691,7 +7708,7 @@
       <c r="E37" t="s">
         <v>452</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="1" t="s">
         <v>453</v>
       </c>
       <c r="G37" t="s">
@@ -7718,7 +7735,7 @@
       <c r="N37" t="s">
         <v>456</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="1" t="s">
         <v>179</v>
       </c>
       <c r="P37" t="s">
@@ -7729,7 +7746,7 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>2248</v>
       </c>
       <c r="B38" t="s">
@@ -7744,7 +7761,7 @@
       <c r="E38" t="s">
         <v>461</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>40922</v>
       </c>
       <c r="G38" t="s">
@@ -7779,7 +7796,7 @@
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>2250</v>
       </c>
       <c r="B39" t="s">
@@ -7794,7 +7811,7 @@
       <c r="E39" t="s">
         <v>469</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="1" t="s">
         <v>470</v>
       </c>
       <c r="G39" t="s">
@@ -7818,7 +7835,7 @@
       <c r="M39" t="s">
         <v>474</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="1" t="s">
         <v>475</v>
       </c>
       <c r="P39" t="s">
@@ -7829,7 +7846,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>2252</v>
       </c>
       <c r="B40" t="s">
@@ -7844,7 +7861,7 @@
       <c r="E40" t="s">
         <v>480</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>27700</v>
       </c>
       <c r="G40" t="s">
@@ -7871,7 +7888,7 @@
       <c r="N40" t="s">
         <v>483</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O40" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P40" t="s">
@@ -7879,7 +7896,7 @@
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>2254</v>
       </c>
       <c r="B41" t="s">
@@ -7894,7 +7911,7 @@
       <c r="E41" t="s">
         <v>488</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>725172</v>
       </c>
       <c r="G41" t="s">
@@ -7921,7 +7938,7 @@
       <c r="N41" t="s">
         <v>491</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O41" s="1" t="s">
         <v>492</v>
       </c>
       <c r="P41" t="s">
@@ -7929,7 +7946,7 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>2256</v>
       </c>
       <c r="B42" t="s">
@@ -7944,7 +7961,7 @@
       <c r="E42" t="s">
         <v>496</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>5577</v>
       </c>
       <c r="G42" t="s">
@@ -7968,7 +7985,7 @@
       <c r="M42" t="s">
         <v>178</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O42" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P42" t="s">
@@ -7979,7 +7996,7 @@
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>2258</v>
       </c>
       <c r="B43" t="s">
@@ -7994,7 +8011,7 @@
       <c r="E43" t="s">
         <v>504</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>83848</v>
       </c>
       <c r="G43" t="s">
@@ -8021,7 +8038,7 @@
       <c r="N43" t="s">
         <v>349</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O43" s="1" t="s">
         <v>507</v>
       </c>
       <c r="P43" t="s">
@@ -8032,7 +8049,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>2260</v>
       </c>
       <c r="B44" t="s">
@@ -8047,7 +8064,7 @@
       <c r="E44" t="s">
         <v>512</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>8109</v>
       </c>
       <c r="G44" t="s">
@@ -8074,7 +8091,7 @@
       <c r="N44" t="s">
         <v>515</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O44" s="1" t="s">
         <v>516</v>
       </c>
       <c r="P44" t="s">
@@ -8085,7 +8102,7 @@
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="1">
         <v>2262</v>
       </c>
       <c r="B45" t="s">
@@ -8100,7 +8117,7 @@
       <c r="E45" t="s">
         <v>521</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>18558</v>
       </c>
       <c r="G45" t="s">
@@ -8127,7 +8144,7 @@
       <c r="N45" t="s">
         <v>286</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O45" s="1" t="s">
         <v>523</v>
       </c>
       <c r="P45" t="s">
@@ -8138,7 +8155,7 @@
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="1">
         <v>2264</v>
       </c>
       <c r="B46" t="s">
@@ -8153,7 +8170,7 @@
       <c r="E46" t="s">
         <v>528</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>20804</v>
       </c>
       <c r="G46" t="s">
@@ -8180,7 +8197,7 @@
       <c r="N46" t="s">
         <v>531</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="1" t="s">
         <v>532</v>
       </c>
       <c r="P46" t="s">
@@ -8188,7 +8205,7 @@
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="1">
         <v>2266</v>
       </c>
       <c r="B47" t="s">
@@ -8203,7 +8220,7 @@
       <c r="E47" t="s">
         <v>536</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="1" t="s">
         <v>537</v>
       </c>
       <c r="G47" t="s">
@@ -8235,7 +8252,7 @@
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="1">
         <v>2268</v>
       </c>
       <c r="B48" t="s">
@@ -8250,7 +8267,7 @@
       <c r="E48" t="s">
         <v>543</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>26097</v>
       </c>
       <c r="G48" t="s">
@@ -8279,7 +8296,7 @@
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="1">
         <v>2270</v>
       </c>
       <c r="B49" t="s">
@@ -8294,7 +8311,7 @@
       <c r="E49" t="s">
         <v>550</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>27729</v>
       </c>
       <c r="G49" t="s">
@@ -8318,7 +8335,7 @@
       <c r="M49" t="s">
         <v>553</v>
       </c>
-      <c r="O49" t="s">
+      <c r="O49" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P49" t="s">
@@ -8329,7 +8346,7 @@
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="1">
         <v>2272</v>
       </c>
       <c r="B50" t="s">
@@ -8344,7 +8361,7 @@
       <c r="E50" t="s">
         <v>558</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>42200</v>
       </c>
       <c r="G50" t="s">
@@ -8379,7 +8396,7 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="1">
         <v>2274</v>
       </c>
       <c r="B51" t="s">
@@ -8394,7 +8411,7 @@
       <c r="E51" t="s">
         <v>567</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <v>60617</v>
       </c>
       <c r="G51" t="s">
@@ -8418,7 +8435,7 @@
       <c r="N51" t="s">
         <v>276</v>
       </c>
-      <c r="O51" t="s">
+      <c r="O51" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P51" t="s">
@@ -8429,7 +8446,7 @@
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="1">
         <v>2276</v>
       </c>
       <c r="B52" t="s">
@@ -8444,7 +8461,7 @@
       <c r="E52" t="s">
         <v>574</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>77940</v>
       </c>
       <c r="G52" t="s">
@@ -8471,7 +8488,7 @@
       <c r="N52" t="s">
         <v>578</v>
       </c>
-      <c r="O52" t="s">
+      <c r="O52" s="1" t="s">
         <v>579</v>
       </c>
       <c r="P52" t="s">
@@ -8482,7 +8499,7 @@
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="1">
         <v>2278</v>
       </c>
       <c r="B53" t="s">
@@ -8497,7 +8514,7 @@
       <c r="E53" t="s">
         <v>584</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <v>722378</v>
       </c>
       <c r="G53" t="s">
@@ -8521,7 +8538,7 @@
       <c r="N53" t="s">
         <v>130</v>
       </c>
-      <c r="O53" t="s">
+      <c r="O53" s="1" t="s">
         <v>587</v>
       </c>
       <c r="P53" t="s">
@@ -8532,7 +8549,7 @@
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54">
+      <c r="A54" s="1">
         <v>2280</v>
       </c>
       <c r="B54" t="s">
@@ -8547,7 +8564,7 @@
       <c r="E54" t="s">
         <v>592</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <v>5164</v>
       </c>
       <c r="G54" t="s">
@@ -8574,7 +8591,7 @@
       <c r="N54" t="s">
         <v>418</v>
       </c>
-      <c r="O54" t="s">
+      <c r="O54" s="1" t="s">
         <v>594</v>
       </c>
       <c r="P54" t="s">
@@ -8585,7 +8602,7 @@
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="1">
         <v>2282</v>
       </c>
       <c r="B55" t="s">
@@ -8600,7 +8617,7 @@
       <c r="E55" t="s">
         <v>598</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="1" t="s">
         <v>599</v>
       </c>
       <c r="G55" t="s">
@@ -8624,7 +8641,7 @@
       <c r="N55" t="s">
         <v>255</v>
       </c>
-      <c r="O55" t="s">
+      <c r="O55" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P55" t="s">
@@ -8635,7 +8652,7 @@
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="1">
         <v>2284</v>
       </c>
       <c r="B56" t="s">
@@ -8650,7 +8667,7 @@
       <c r="E56" t="s">
         <v>606</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>579427</v>
       </c>
       <c r="G56" t="s">
@@ -8677,7 +8694,7 @@
       <c r="N56" t="s">
         <v>609</v>
       </c>
-      <c r="O56" t="s">
+      <c r="O56" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P56" t="s">
@@ -8688,7 +8705,7 @@
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="1">
         <v>2286</v>
       </c>
       <c r="B57" t="s">
@@ -8703,7 +8720,7 @@
       <c r="E57" t="s">
         <v>614</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <v>982273</v>
       </c>
       <c r="G57" t="s">
@@ -8730,7 +8747,7 @@
       <c r="N57" t="s">
         <v>418</v>
       </c>
-      <c r="O57" t="s">
+      <c r="O57" s="1" t="s">
         <v>618</v>
       </c>
       <c r="P57" t="s">
@@ -8741,7 +8758,7 @@
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="1">
         <v>2288</v>
       </c>
       <c r="B58" t="s">
@@ -8756,7 +8773,7 @@
       <c r="E58" t="s">
         <v>623</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="1" t="s">
         <v>624</v>
       </c>
       <c r="G58" t="s">
@@ -8783,7 +8800,7 @@
       <c r="N58" t="s">
         <v>626</v>
       </c>
-      <c r="O58" t="s">
+      <c r="O58" s="1" t="s">
         <v>627</v>
       </c>
       <c r="P58" t="s">
@@ -8794,7 +8811,7 @@
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="1">
         <v>2290</v>
       </c>
       <c r="B59" t="s">
@@ -8809,7 +8826,7 @@
       <c r="E59" t="s">
         <v>632</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>682358</v>
       </c>
       <c r="G59" t="s">
@@ -8833,7 +8850,7 @@
       <c r="N59" t="s">
         <v>286</v>
       </c>
-      <c r="O59" t="s">
+      <c r="O59" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P59" t="s">
@@ -8844,7 +8861,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="1">
         <v>2292</v>
       </c>
       <c r="B60" t="s">
@@ -8859,7 +8876,7 @@
       <c r="E60" t="s">
         <v>638</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="1" t="s">
         <v>639</v>
       </c>
       <c r="G60" t="s">
@@ -8888,7 +8905,7 @@
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="1">
         <v>2294</v>
       </c>
       <c r="B61" t="s">
@@ -8903,7 +8920,7 @@
       <c r="E61" t="s">
         <v>646</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>2552</v>
       </c>
       <c r="G61" t="s">
@@ -8927,7 +8944,7 @@
       <c r="M61" t="s">
         <v>648</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O61" s="1" t="s">
         <v>649</v>
       </c>
       <c r="P61" t="s">
@@ -8938,7 +8955,7 @@
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="1">
         <v>2296</v>
       </c>
       <c r="B62" t="s">
@@ -8953,7 +8970,7 @@
       <c r="E62" t="s">
         <v>654</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="1" t="s">
         <v>655</v>
       </c>
       <c r="G62" t="s">
@@ -8980,7 +8997,7 @@
       <c r="N62" t="s">
         <v>456</v>
       </c>
-      <c r="O62" t="s">
+      <c r="O62" s="1" t="s">
         <v>658</v>
       </c>
       <c r="P62" t="s">
@@ -8988,7 +9005,7 @@
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="1">
         <v>2298</v>
       </c>
       <c r="B63" t="s">
@@ -9003,7 +9020,7 @@
       <c r="E63" t="s">
         <v>662</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <v>39196</v>
       </c>
       <c r="G63" t="s">
@@ -9027,7 +9044,7 @@
       <c r="N63" t="s">
         <v>130</v>
       </c>
-      <c r="O63" t="s">
+      <c r="O63" s="1" t="s">
         <v>665</v>
       </c>
       <c r="P63" t="s">
@@ -9038,7 +9055,7 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="1">
         <v>2300</v>
       </c>
       <c r="B64" t="s">
@@ -9053,7 +9070,7 @@
       <c r="E64" t="s">
         <v>670</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="1">
         <v>185366</v>
       </c>
       <c r="G64" t="s">
@@ -9080,7 +9097,7 @@
       <c r="N64" t="s">
         <v>674</v>
       </c>
-      <c r="O64" t="s">
+      <c r="O64" s="1" t="s">
         <v>675</v>
       </c>
       <c r="P64" t="s">
@@ -9091,7 +9108,7 @@
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="1">
         <v>2302</v>
       </c>
       <c r="B65" t="s">
@@ -9106,7 +9123,7 @@
       <c r="E65" t="s">
         <v>680</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <v>84558</v>
       </c>
       <c r="G65" t="s">
@@ -9133,7 +9150,7 @@
       <c r="N65" t="s">
         <v>683</v>
       </c>
-      <c r="O65" t="s">
+      <c r="O65" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P65" t="s">
@@ -9144,7 +9161,7 @@
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="1">
         <v>2304</v>
       </c>
       <c r="B66" t="s">
@@ -9159,7 +9176,7 @@
       <c r="E66" t="s">
         <v>688</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <v>50100</v>
       </c>
       <c r="G66" t="s">
@@ -9191,7 +9208,7 @@
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="1">
         <v>2306</v>
       </c>
       <c r="B67" t="s">
@@ -9206,7 +9223,7 @@
       <c r="E67" t="s">
         <v>696</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="1">
         <v>784335</v>
       </c>
       <c r="G67" t="s">
@@ -9230,7 +9247,7 @@
       <c r="N67" t="s">
         <v>515</v>
       </c>
-      <c r="O67" t="s">
+      <c r="O67" s="1" t="s">
         <v>699</v>
       </c>
       <c r="P67" t="s">
@@ -9238,7 +9255,7 @@
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="1">
         <v>2308</v>
       </c>
       <c r="B68" t="s">
@@ -9253,7 +9270,7 @@
       <c r="E68" t="s">
         <v>703</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <v>61400</v>
       </c>
       <c r="G68" t="s">
@@ -9288,7 +9305,7 @@
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="1">
         <v>2310</v>
       </c>
       <c r="B69" t="s">
@@ -9303,7 +9320,7 @@
       <c r="E69" t="s">
         <v>711</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="1">
         <v>20800</v>
       </c>
       <c r="G69" t="s">
@@ -9330,7 +9347,7 @@
       <c r="N69" t="s">
         <v>255</v>
       </c>
-      <c r="O69" t="s">
+      <c r="O69" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P69" t="s">
@@ -9341,7 +9358,7 @@
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="1">
         <v>2312</v>
       </c>
       <c r="B70" t="s">
@@ -9356,7 +9373,7 @@
       <c r="E70" t="s">
         <v>623</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="1">
         <v>495497</v>
       </c>
       <c r="G70" t="s">
@@ -9380,7 +9397,7 @@
       <c r="N70" t="s">
         <v>719</v>
       </c>
-      <c r="O70" t="s">
+      <c r="O70" s="1" t="s">
         <v>499</v>
       </c>
       <c r="P70" t="s">
@@ -9391,7 +9408,7 @@
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A71">
+      <c r="A71" s="1">
         <v>2314</v>
       </c>
       <c r="B71" t="s">
@@ -9406,7 +9423,7 @@
       <c r="E71" t="s">
         <v>724</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="1">
         <v>30365</v>
       </c>
       <c r="G71" t="s">
@@ -9438,7 +9455,7 @@
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A72">
+      <c r="A72" s="1">
         <v>2316</v>
       </c>
       <c r="B72" t="s">
@@ -9453,7 +9470,7 @@
       <c r="E72" t="s">
         <v>732</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="1">
         <v>647071</v>
       </c>
       <c r="G72" t="s">
@@ -9480,7 +9497,7 @@
       <c r="N72" t="s">
         <v>734</v>
       </c>
-      <c r="O72" t="s">
+      <c r="O72" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P72" t="s">
@@ -9491,7 +9508,7 @@
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A73">
+      <c r="A73" s="1">
         <v>2318</v>
       </c>
       <c r="B73" t="s">
@@ -9506,7 +9523,7 @@
       <c r="E73" t="s">
         <v>739</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="1">
         <v>7801</v>
       </c>
       <c r="G73" t="s">
@@ -9530,7 +9547,7 @@
       <c r="M73" t="s">
         <v>188</v>
       </c>
-      <c r="O73" t="s">
+      <c r="O73" s="1" t="s">
         <v>143</v>
       </c>
       <c r="P73" t="s">
@@ -9541,7 +9558,7 @@
       </c>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A74">
+      <c r="A74" s="1">
         <v>2320</v>
       </c>
       <c r="B74" t="s">
@@ -9556,7 +9573,7 @@
       <c r="E74" t="s">
         <v>745</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="1">
         <v>6472</v>
       </c>
       <c r="G74" t="s">
@@ -9582,7 +9599,7 @@
       </c>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A75">
+      <c r="A75" s="1">
         <v>2322</v>
       </c>
       <c r="B75" t="s">
@@ -9597,7 +9614,7 @@
       <c r="E75" t="s">
         <v>751</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="1" t="s">
         <v>752</v>
       </c>
       <c r="G75" t="s">
@@ -9624,7 +9641,7 @@
       <c r="N75" t="s">
         <v>755</v>
       </c>
-      <c r="O75" t="s">
+      <c r="O75" s="1" t="s">
         <v>594</v>
       </c>
       <c r="P75" t="s">
@@ -9635,7 +9652,7 @@
       </c>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A76">
+      <c r="A76" s="1">
         <v>2324</v>
       </c>
       <c r="B76" t="s">
@@ -9650,7 +9667,7 @@
       <c r="E76" t="s">
         <v>760</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="1">
         <v>613813</v>
       </c>
       <c r="G76" t="s">
@@ -9677,7 +9694,7 @@
       <c r="N76" t="s">
         <v>418</v>
       </c>
-      <c r="O76" t="s">
+      <c r="O76" s="1" t="s">
         <v>763</v>
       </c>
       <c r="P76" t="s">
@@ -9688,7 +9705,7 @@
       </c>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A77">
+      <c r="A77" s="1">
         <v>2326</v>
       </c>
       <c r="B77" t="s">
@@ -9703,7 +9720,7 @@
       <c r="E77" t="s">
         <v>768</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="1">
         <v>21600</v>
       </c>
       <c r="G77" t="s">
@@ -9738,7 +9755,7 @@
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A78">
+      <c r="A78" s="1">
         <v>2328</v>
       </c>
       <c r="B78" t="s">
@@ -9753,7 +9770,7 @@
       <c r="E78" t="s">
         <v>776</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="1">
         <v>22930</v>
       </c>
       <c r="G78" t="s">
@@ -9777,7 +9794,7 @@
       <c r="M78" t="s">
         <v>311</v>
       </c>
-      <c r="O78" t="s">
+      <c r="O78" s="1" t="s">
         <v>618</v>
       </c>
       <c r="P78" t="s">
@@ -9788,7 +9805,7 @@
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A79">
+      <c r="A79" s="1">
         <v>2330</v>
       </c>
       <c r="B79" t="s">
@@ -9803,7 +9820,7 @@
       <c r="E79" t="s">
         <v>783</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="1">
         <v>18648</v>
       </c>
       <c r="G79" t="s">
@@ -9830,7 +9847,7 @@
       <c r="N79" t="s">
         <v>786</v>
       </c>
-      <c r="O79" t="s">
+      <c r="O79" s="1" t="s">
         <v>516</v>
       </c>
       <c r="P79" t="s">
@@ -9841,7 +9858,7 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A80">
+      <c r="A80" s="1">
         <v>2332</v>
       </c>
       <c r="B80" t="s">
@@ -9856,7 +9873,7 @@
       <c r="E80" t="s">
         <v>790</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="1" t="s">
         <v>791</v>
       </c>
       <c r="G80" t="s">
@@ -9885,7 +9902,7 @@
       </c>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81">
+      <c r="A81" s="1">
         <v>2334</v>
       </c>
       <c r="B81" t="s">
@@ -9900,7 +9917,7 @@
       <c r="E81" t="s">
         <v>796</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="1">
         <v>60175</v>
       </c>
       <c r="G81" t="s">
@@ -9932,7 +9949,7 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82">
+      <c r="A82" s="1">
         <v>2336</v>
       </c>
       <c r="B82" t="s">
@@ -9947,7 +9964,7 @@
       <c r="E82" t="s">
         <v>802</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="1">
         <v>13427</v>
       </c>
       <c r="G82" t="s">
@@ -9971,7 +9988,7 @@
       <c r="M82" t="s">
         <v>805</v>
       </c>
-      <c r="O82" t="s">
+      <c r="O82" s="1" t="s">
         <v>484</v>
       </c>
       <c r="P82" t="s">
@@ -9982,7 +9999,7 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83">
+      <c r="A83" s="1">
         <v>2338</v>
       </c>
       <c r="B83" t="s">
@@ -9997,7 +10014,7 @@
       <c r="E83" t="s">
         <v>623</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="1" t="s">
         <v>810</v>
       </c>
       <c r="G83" t="s">
@@ -10024,7 +10041,7 @@
       <c r="N83" t="s">
         <v>531</v>
       </c>
-      <c r="O83" t="s">
+      <c r="O83" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P83" t="s">
@@ -10035,7 +10052,7 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84">
+      <c r="A84" s="1">
         <v>2340</v>
       </c>
       <c r="B84" t="s">
@@ -10050,7 +10067,7 @@
       <c r="E84" t="s">
         <v>817</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="1">
         <v>15388</v>
       </c>
       <c r="G84" t="s">
@@ -10077,7 +10094,7 @@
       <c r="N84" t="s">
         <v>820</v>
       </c>
-      <c r="O84" t="s">
+      <c r="O84" s="1" t="s">
         <v>821</v>
       </c>
       <c r="P84" t="s">
@@ -10088,7 +10105,7 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85">
+      <c r="A85" s="1">
         <v>2342</v>
       </c>
       <c r="B85" t="s">
@@ -10103,7 +10120,7 @@
       <c r="E85" t="s">
         <v>826</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="1">
         <v>763583</v>
       </c>
       <c r="G85" t="s">
@@ -10130,7 +10147,7 @@
       <c r="N85" t="s">
         <v>829</v>
       </c>
-      <c r="O85" t="s">
+      <c r="O85" s="1" t="s">
         <v>830</v>
       </c>
       <c r="P85" t="s">
@@ -10138,7 +10155,7 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86">
+      <c r="A86" s="1">
         <v>2344</v>
       </c>
       <c r="B86" t="s">
@@ -10153,7 +10170,7 @@
       <c r="E86" t="s">
         <v>834</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="1">
         <v>21505</v>
       </c>
       <c r="G86" t="s">
@@ -10180,7 +10197,7 @@
       <c r="N86" t="s">
         <v>515</v>
       </c>
-      <c r="O86" t="s">
+      <c r="O86" s="1" t="s">
         <v>837</v>
       </c>
       <c r="P86" t="s">
@@ -10191,7 +10208,7 @@
       </c>
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A87">
+      <c r="A87" s="1">
         <v>2346</v>
       </c>
       <c r="B87" t="s">
@@ -10206,7 +10223,7 @@
       <c r="E87" t="s">
         <v>842</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="1">
         <v>854349</v>
       </c>
       <c r="G87" t="s">
@@ -10233,7 +10250,7 @@
       <c r="N87" t="s">
         <v>578</v>
       </c>
-      <c r="O87" t="s">
+      <c r="O87" s="1" t="s">
         <v>844</v>
       </c>
       <c r="P87" t="s">
@@ -10244,7 +10261,7 @@
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A88">
+      <c r="A88" s="1">
         <v>2348</v>
       </c>
       <c r="B88" t="s">
@@ -10259,7 +10276,7 @@
       <c r="E88" t="s">
         <v>849</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="1">
         <v>99479</v>
       </c>
       <c r="G88" t="s">
@@ -10286,7 +10303,7 @@
       <c r="N88" t="s">
         <v>276</v>
       </c>
-      <c r="O88" t="s">
+      <c r="O88" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P88" t="s">
@@ -10297,7 +10314,7 @@
       </c>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A89">
+      <c r="A89" s="1">
         <v>2350</v>
       </c>
       <c r="B89" t="s">
@@ -10312,7 +10329,7 @@
       <c r="E89" t="s">
         <v>855</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="1">
         <v>39926</v>
       </c>
       <c r="G89" t="s">
@@ -10336,7 +10353,7 @@
       <c r="N89" t="s">
         <v>857</v>
       </c>
-      <c r="O89" t="s">
+      <c r="O89" s="1" t="s">
         <v>858</v>
       </c>
       <c r="P89" t="s">
@@ -10347,7 +10364,7 @@
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A90">
+      <c r="A90" s="1">
         <v>2352</v>
       </c>
       <c r="B90" t="s">
@@ -10362,7 +10379,7 @@
       <c r="E90" t="s">
         <v>863</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="1">
         <v>956033</v>
       </c>
       <c r="G90" t="s">
@@ -10389,7 +10406,7 @@
       <c r="N90" t="s">
         <v>866</v>
       </c>
-      <c r="O90" t="s">
+      <c r="O90" s="1" t="s">
         <v>342</v>
       </c>
       <c r="P90" t="s">
@@ -10400,7 +10417,7 @@
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A91">
+      <c r="A91" s="1">
         <v>2354</v>
       </c>
       <c r="B91" t="s">
@@ -10415,7 +10432,7 @@
       <c r="E91" t="s">
         <v>871</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="1">
         <v>27729</v>
       </c>
       <c r="G91" t="s">
@@ -10442,7 +10459,7 @@
       <c r="N91" t="s">
         <v>873</v>
       </c>
-      <c r="O91" t="s">
+      <c r="O91" s="1" t="s">
         <v>155</v>
       </c>
       <c r="P91" t="s">
@@ -10453,7 +10470,7 @@
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A92">
+      <c r="A92" s="1">
         <v>2356</v>
       </c>
       <c r="B92" t="s">
@@ -10468,7 +10485,7 @@
       <c r="E92" t="s">
         <v>877</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="1">
         <v>16704</v>
       </c>
       <c r="G92" t="s">
@@ -10492,7 +10509,7 @@
       <c r="N92" t="s">
         <v>880</v>
       </c>
-      <c r="O92" t="s">
+      <c r="O92" s="1" t="s">
         <v>287</v>
       </c>
       <c r="P92" t="s">
@@ -10500,7 +10517,7 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93">
+      <c r="A93" s="1">
         <v>2358</v>
       </c>
       <c r="B93" t="s">
@@ -10515,7 +10532,7 @@
       <c r="E93" t="s">
         <v>884</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="1">
         <v>4932</v>
       </c>
       <c r="G93" t="s">
@@ -10539,7 +10556,7 @@
       <c r="M93" t="s">
         <v>188</v>
       </c>
-      <c r="O93" t="s">
+      <c r="O93" s="1" t="s">
         <v>658</v>
       </c>
       <c r="P93" t="s">
@@ -10550,7 +10567,7 @@
       </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94">
+      <c r="A94" s="1">
         <v>2360</v>
       </c>
       <c r="B94" t="s">
@@ -10565,7 +10582,7 @@
       <c r="E94" t="s">
         <v>891</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="1">
         <v>969734</v>
       </c>
       <c r="G94" t="s">
@@ -10600,7 +10617,7 @@
       </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A95">
+      <c r="A95" s="1">
         <v>2362</v>
       </c>
       <c r="B95" t="s">
@@ -10615,7 +10632,7 @@
       <c r="E95" t="s">
         <v>898</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="1">
         <v>2130</v>
       </c>
       <c r="G95" t="s">
@@ -10642,7 +10659,7 @@
       <c r="N95" t="s">
         <v>515</v>
       </c>
-      <c r="O95" t="s">
+      <c r="O95" s="1" t="s">
         <v>901</v>
       </c>
       <c r="P95" t="s">
@@ -10650,7 +10667,7 @@
       </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96">
+      <c r="A96" s="1">
         <v>2364</v>
       </c>
       <c r="B96" t="s">
@@ -10665,7 +10682,7 @@
       <c r="E96" t="s">
         <v>905</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="1">
         <v>8145</v>
       </c>
       <c r="G96" t="s">
@@ -10694,7 +10711,7 @@
       </c>
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A97">
+      <c r="A97" s="1">
         <v>2366</v>
       </c>
       <c r="B97" t="s">
@@ -10709,7 +10726,7 @@
       <c r="E97" t="s">
         <v>912</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="1" t="s">
         <v>913</v>
       </c>
       <c r="G97" t="s">
@@ -10736,7 +10753,7 @@
       <c r="N97" t="s">
         <v>276</v>
       </c>
-      <c r="O97" t="s">
+      <c r="O97" s="1" t="s">
         <v>916</v>
       </c>
       <c r="P97" t="s">
@@ -10747,7 +10764,7 @@
       </c>
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A98">
+      <c r="A98" s="1">
         <v>2368</v>
       </c>
       <c r="B98" t="s">
@@ -10762,7 +10779,7 @@
       <c r="E98" t="s">
         <v>921</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="1">
         <v>823823</v>
       </c>
       <c r="G98" t="s">
@@ -10786,7 +10803,7 @@
       <c r="M98" t="s">
         <v>254</v>
       </c>
-      <c r="O98" t="s">
+      <c r="O98" s="1" t="s">
         <v>532</v>
       </c>
       <c r="P98" t="s">
@@ -10797,7 +10814,7 @@
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A99">
+      <c r="A99" s="1">
         <v>2370</v>
       </c>
       <c r="B99" t="s">
@@ -10812,7 +10829,7 @@
       <c r="E99" t="s">
         <v>927</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="1">
         <v>583509</v>
       </c>
       <c r="G99" t="s">
@@ -10836,7 +10853,7 @@
       <c r="M99" t="s">
         <v>196</v>
       </c>
-      <c r="O99" t="s">
+      <c r="O99" s="1" t="s">
         <v>930</v>
       </c>
       <c r="P99" t="s">
@@ -10844,7 +10861,7 @@
       </c>
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A100">
+      <c r="A100" s="1">
         <v>2372</v>
       </c>
       <c r="B100" t="s">
@@ -10859,7 +10876,7 @@
       <c r="E100" t="s">
         <v>934</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="1">
         <v>588185</v>
       </c>
       <c r="G100" t="s">
@@ -10883,7 +10900,7 @@
       <c r="N100" t="s">
         <v>873</v>
       </c>
-      <c r="O100" t="s">
+      <c r="O100" s="1" t="s">
         <v>937</v>
       </c>
       <c r="P100" t="s">
@@ -10894,7 +10911,7 @@
       </c>
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A101">
+      <c r="A101" s="1">
         <v>2374</v>
       </c>
       <c r="B101" t="s">
@@ -10909,7 +10926,7 @@
       <c r="E101" t="s">
         <v>942</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="1">
         <v>7053</v>
       </c>
       <c r="G101" t="s">
@@ -10936,7 +10953,7 @@
       <c r="N101" t="s">
         <v>945</v>
       </c>
-      <c r="O101" t="s">
+      <c r="O101" s="1" t="s">
         <v>235</v>
       </c>
       <c r="P101" t="s">
@@ -18670,7 +18687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89A6CDD-DBCC-584C-89E0-70AF5717A48B}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>

</xml_diff>